<commit_message>
bisa delte dan update password
</commit_message>
<xml_diff>
--- a/list feature.xlsx
+++ b/list feature.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>controller</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>download file</t>
+  </si>
+  <si>
+    <t>manage uploaded file</t>
+  </si>
+  <si>
+    <t>enkripsi</t>
   </si>
 </sst>
 </file>
@@ -424,16 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96911BF4-335E-4AE1-898C-DA67F96F0CF8}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,13 +485,24 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>14</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -499,26 +516,43 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="C11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>